<commit_message>
Update excel export import
</commit_message>
<xml_diff>
--- a/public/templat/Templat-Masukan-Vendor.xlsx
+++ b/public/templat/Templat-Masukan-Vendor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Kerja\Sandra-RC\public\templat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53A6214-7529-4F1D-A46B-6A29D40150E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE23853B-2541-4DD8-8C59-B8B137FE5737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88BF9555-E7E4-144F-B65F-456652F0C5A3}"/>
   </bookViews>
@@ -152,10 +152,10 @@
     <t>*)  Masukkan dengan format nomor, EX : 1,4,5</t>
   </si>
   <si>
-    <t>Asac</t>
-  </si>
-  <si>
-    <t>VVxsf</t>
+    <t>Vendor Satu</t>
+  </si>
+  <si>
+    <t>Vendor Dua</t>
   </si>
 </sst>
 </file>
@@ -212,12 +212,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,6 +227,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +550,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -595,13 +600,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -613,7 +618,7 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>123133</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -627,13 +632,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -645,7 +650,7 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>123123</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -683,130 +688,130 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>